<commit_message>
wrong date-time format message edited
</commit_message>
<xml_diff>
--- a/src/Assignment.Description/Nobel_Prize_Winners.xlsx
+++ b/src/Assignment.Description/Nobel_Prize_Winners.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5915" uniqueCount="2474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5919" uniqueCount="2478">
   <si>
     <t>Year</t>
   </si>
@@ -7441,6 +7441,18 @@
   </si>
   <si>
     <t>iuh</t>
+  </si>
+  <si>
+    <t>dada</t>
+  </si>
+  <si>
+    <t>r23e</t>
+  </si>
+  <si>
+    <t>dadadad</t>
+  </si>
+  <si>
+    <t>12qwas</t>
   </si>
 </sst>
 </file>
@@ -8307,7 +8319,7 @@
   <dimension ref="A1:K807"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A791" workbookViewId="0">
-      <selection activeCell="A801" sqref="A801:XFD801"/>
+      <selection activeCell="D805" sqref="D805"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31486,6 +31498,11 @@
         <v>379</v>
       </c>
     </row>
+    <row r="801" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D801" t="s">
+        <v>2474</v>
+      </c>
+    </row>
     <row r="802" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A802">
         <v>2</v>
@@ -31496,6 +31513,9 @@
       <c r="C802" t="s">
         <v>921</v>
       </c>
+      <c r="D802" t="s">
+        <v>2475</v>
+      </c>
       <c r="I802" t="s">
         <v>30</v>
       </c>
@@ -31513,6 +31533,9 @@
       <c r="C803" t="s">
         <v>1188</v>
       </c>
+      <c r="D803" t="s">
+        <v>2476</v>
+      </c>
       <c r="I803" t="s">
         <v>48</v>
       </c>
@@ -31561,6 +31584,9 @@
       </c>
       <c r="C805" t="s">
         <v>55</v>
+      </c>
+      <c r="D805" t="s">
+        <v>2477</v>
       </c>
       <c r="E805" t="s">
         <v>56</v>

</xml_diff>